<commit_message>
refactor code and delete useless funcs
</commit_message>
<xml_diff>
--- a/btg.xlsx
+++ b/btg.xlsx
@@ -12906,124 +12906,108 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>PLUG INVEST AGENTE AUTONOMO DE INVESTIMENTOS S/S LTDA</t>
+          <t>PRANA INVESTIMENTOS AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 29.724.240/0001-10 </t>
+          <t xml:space="preserve"> 31.199.764/0001-81 </t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t xml:space="preserve"> investimentos@pluginvestimentos.com.br </t>
+          <t xml:space="preserve"> contato@pranainvestimentos.com </t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>Rua Lauro Linhares, 2010, Sala 709 - Bloco A</t>
+          <t>Rua Professor Atilio Innocenti, 474 - cj 801</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>(48) 3207-6579</t>
+          <t>(11) 4861-1838</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SC </t>
+          <t xml:space="preserve"> SP </t>
         </is>
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t xml:space="preserve"> https://pranainvestimentos.com/ </t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
         <is>
-          <t>Florianópolis</t>
+          <t>São Paulo</t>
         </is>
       </c>
       <c r="I226" t="inlineStr">
         <is>
-          <t>07/02/2022</t>
+          <t>01/02/2021</t>
         </is>
       </c>
       <c r="J226" t="inlineStr">
         <is>
-          <t>Trindade</t>
+          <t>Vila Nova Conceição</t>
         </is>
       </c>
       <c r="K226" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 88036-002 </t>
+          <t xml:space="preserve"> 04538-001 </t>
         </is>
       </c>
       <c r="L226" t="inlineStr">
         <is>
-          <t>JOÃO FELIPE DA SILVA FRANDOLOZO</t>
+          <t>BRUNO HARDT FREITAS DE SOUZA</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>PRANA INVESTIMENTOS AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
-        </is>
-      </c>
-      <c r="B227" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 31.199.764/0001-81 </t>
-        </is>
-      </c>
-      <c r="C227" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> contato@pranainvestimentos.com </t>
-        </is>
-      </c>
+          <t>PROFITTO AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr"/>
+      <c r="C227" t="inlineStr"/>
       <c r="D227" t="inlineStr">
         <is>
-          <t>Rua Professor Atilio Innocenti, 474 - cj 801</t>
-        </is>
-      </c>
-      <c r="E227" t="inlineStr">
-        <is>
-          <t>(11) 4861-1838</t>
-        </is>
-      </c>
+          <t>Avenida Benjamin, nº316, sala1004, Edificio Vesta</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr"/>
       <c r="F227" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SP </t>
+          <t xml:space="preserve"> RS </t>
         </is>
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://pranainvestimentos.com/ </t>
+          <t xml:space="preserve"> - </t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
         <is>
-          <t>São Paulo</t>
-        </is>
-      </c>
-      <c r="I227" t="inlineStr">
-        <is>
-          <t>01/02/2021</t>
-        </is>
-      </c>
+          <t>Torres</t>
+        </is>
+      </c>
+      <c r="I227" t="inlineStr"/>
       <c r="J227" t="inlineStr">
         <is>
-          <t>Vila Nova Conceição</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="K227" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 04538-001 </t>
+          <t xml:space="preserve"> 95560-000 </t>
         </is>
       </c>
       <c r="L227" t="inlineStr">
         <is>
-          <t>BRUNO HARDT FREITAS DE SOUZA</t>
+          <t>Marcos Meneghetti</t>
         </is>
       </c>
     </row>
@@ -13033,14 +13017,26 @@
           <t>PROFITTO AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
         </is>
       </c>
-      <c r="B228" t="inlineStr"/>
-      <c r="C228" t="inlineStr"/>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 41.148.237/0001-00 </t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> marcos@profittoinvestimentos.com.br </t>
+        </is>
+      </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>Avenida Benjamin, nº316, sala1004, Edificio Vesta</t>
-        </is>
-      </c>
-      <c r="E228" t="inlineStr"/>
+          <t>Av. Dr. Nilo Peçanha, 2900, sala 803</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>(51) 3303-3873</t>
+        </is>
+      </c>
       <c r="F228" t="inlineStr">
         <is>
           <t xml:space="preserve"> RS </t>
@@ -13053,18 +13049,22 @@
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>Torres</t>
-        </is>
-      </c>
-      <c r="I228" t="inlineStr"/>
+          <t>Porto Alegre</t>
+        </is>
+      </c>
+      <c r="I228" t="inlineStr">
+        <is>
+          <t>16/04/2021</t>
+        </is>
+      </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Petrópolis</t>
         </is>
       </c>
       <c r="K228" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 95560-000 </t>
+          <t xml:space="preserve"> 91330-001 </t>
         </is>
       </c>
       <c r="L228" t="inlineStr">
@@ -13076,27 +13076,27 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>PROFITTO AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
+          <t>PROPOSITO CAPITAL AGENTE AUTONOMOS DE INVESTIMENTO EIRELI</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 41.148.237/0001-00 </t>
+          <t xml:space="preserve"> 38.075.724/0001-77 </t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t xml:space="preserve"> marcos@profittoinvestimentos.com.br </t>
+          <t xml:space="preserve"> jdc@proposito-cap.com </t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>Av. Dr. Nilo Peçanha, 2900, sala 803</t>
+          <t>Rua Carlos Von Koseritz, 1200, apt 704</t>
         </is>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>(51) 3303-3873</t>
+          <t>(51) 9333-1468</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -13116,49 +13116,49 @@
       </c>
       <c r="I229" t="inlineStr">
         <is>
-          <t>16/04/2021</t>
+          <t>08/02/2021</t>
         </is>
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>Petrópolis</t>
+          <t>São João</t>
         </is>
       </c>
       <c r="K229" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 91330-001 </t>
+          <t xml:space="preserve"> 90540-030 </t>
         </is>
       </c>
       <c r="L229" t="inlineStr">
         <is>
-          <t>Marcos Meneghetti</t>
+          <t>JULIA PANTE DE CESARO</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>PROPOSITO CAPITAL AGENTE AUTONOMOS DE INVESTIMENTO EIRELI</t>
+          <t>PVI AGENTE AUTONOMO DE INVESTIMENTOS EIRELI</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 38.075.724/0001-77 </t>
+          <t xml:space="preserve"> 08.642.713/0001-60 </t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t xml:space="preserve"> jdc@proposito-cap.com </t>
+          <t xml:space="preserve"> pvi@pviinvestimentos.com.br </t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>Rua Carlos Von Koseritz, 1200, apt 704</t>
+          <t>Avenida Coronel Lucas de Oliveira, 1155 - apt 701</t>
         </is>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>(51) 9333-1468</t>
+          <t>(11) 2827-3910</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -13168,7 +13168,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t xml:space="preserve"> http://pviinvestimentos.com.br/ </t>
         </is>
       </c>
       <c r="H230" t="inlineStr">
@@ -13178,84 +13178,68 @@
       </c>
       <c r="I230" t="inlineStr">
         <is>
-          <t>08/02/2021</t>
+          <t>27/02/2020</t>
         </is>
       </c>
       <c r="J230" t="inlineStr">
         <is>
-          <t>São João</t>
+          <t>Petrópolis</t>
         </is>
       </c>
       <c r="K230" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 90540-030 </t>
+          <t xml:space="preserve"> 90440-011 </t>
         </is>
       </c>
       <c r="L230" t="inlineStr">
         <is>
-          <t>JULIA PANTE DE CESARO</t>
+          <t>Raquel Batista Ourique Cairoli</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>PVI AGENTE AUTONOMO DE INVESTIMENTOS EIRELI</t>
-        </is>
-      </c>
-      <c r="B231" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 08.642.713/0001-60 </t>
-        </is>
-      </c>
-      <c r="C231" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> pvi@pviinvestimentos.com.br </t>
-        </is>
-      </c>
+          <t>POTENZA AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr"/>
+      <c r="C231" t="inlineStr"/>
       <c r="D231" t="inlineStr">
         <is>
-          <t>Avenida Coronel Lucas de Oliveira, 1155 - apt 701</t>
-        </is>
-      </c>
-      <c r="E231" t="inlineStr">
-        <is>
-          <t>(11) 2827-3910</t>
-        </is>
-      </c>
+          <t>Avenida Cassiano Ricardo, nº 319, Sala 1805</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr"/>
       <c r="F231" t="inlineStr">
         <is>
-          <t xml:space="preserve"> RS </t>
+          <t xml:space="preserve"> SP </t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t xml:space="preserve"> http://pviinvestimentos.com.br/ </t>
+          <t xml:space="preserve"> - </t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
-        </is>
-      </c>
-      <c r="I231" t="inlineStr">
-        <is>
-          <t>27/02/2020</t>
-        </is>
-      </c>
+          <t>São José dos Campos</t>
+        </is>
+      </c>
+      <c r="I231" t="inlineStr"/>
       <c r="J231" t="inlineStr">
         <is>
-          <t>Petrópolis</t>
+          <t>Parque Residencial Aquarius</t>
         </is>
       </c>
       <c r="K231" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 90440-011 </t>
+          <t xml:space="preserve"> 12246-870 </t>
         </is>
       </c>
       <c r="L231" t="inlineStr">
         <is>
-          <t>Raquel Batista Ourique Cairoli</t>
+          <t>Gabriel Pinheiro Marto Rodrigues</t>
         </is>
       </c>
     </row>
@@ -13269,7 +13253,7 @@
       <c r="C232" t="inlineStr"/>
       <c r="D232" t="inlineStr">
         <is>
-          <t>Avenida Cassiano Ricardo, nº 319, Sala 1805</t>
+          <t>Saldanha Marinho, nº 1120</t>
         </is>
       </c>
       <c r="E232" t="inlineStr"/>
@@ -13285,18 +13269,18 @@
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>Piracicaba</t>
         </is>
       </c>
       <c r="I232" t="inlineStr"/>
       <c r="J232" t="inlineStr">
         <is>
-          <t>Parque Residencial Aquarius</t>
+          <t>Cidade Jardim</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 12246-870 </t>
+          <t xml:space="preserve"> 13416-320 </t>
         </is>
       </c>
       <c r="L232" t="inlineStr">
@@ -13315,7 +13299,7 @@
       <c r="C233" t="inlineStr"/>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Saldanha Marinho, nº 1120</t>
+          <t>Rua Passeio dos Ipês, nº 320, sala 107, Condominio Tríade</t>
         </is>
       </c>
       <c r="E233" t="inlineStr"/>
@@ -13331,18 +13315,18 @@
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>Piracicaba</t>
+          <t>São Carlos</t>
         </is>
       </c>
       <c r="I233" t="inlineStr"/>
       <c r="J233" t="inlineStr">
         <is>
-          <t>Cidade Jardim</t>
+          <t>Parque Faber Castell I</t>
         </is>
       </c>
       <c r="K233" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 13416-320 </t>
+          <t xml:space="preserve"> 13561-385 </t>
         </is>
       </c>
       <c r="L233" t="inlineStr">
@@ -13357,14 +13341,26 @@
           <t>POTENZA AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
         </is>
       </c>
-      <c r="B234" t="inlineStr"/>
-      <c r="C234" t="inlineStr"/>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 29.936.830/0001-07 </t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> contato@potenzacapital.com.br </t>
+        </is>
+      </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>Rua Passeio dos Ipês, nº 320, sala 107, Condominio Tríade</t>
-        </is>
-      </c>
-      <c r="E234" t="inlineStr"/>
+          <t>Avenida Presidente Juscelino Kubitschek, nº 360, conjunto 191</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>(11) 3846-7916</t>
+        </is>
+      </c>
       <c r="F234" t="inlineStr">
         <is>
           <t xml:space="preserve"> SP </t>
@@ -13372,90 +13368,78 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t xml:space="preserve"> https://www.potenzacapital.com.br/contato </t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>São Carlos</t>
-        </is>
-      </c>
-      <c r="I234" t="inlineStr"/>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="I234" t="inlineStr">
+        <is>
+          <t>23/07/2020</t>
+        </is>
+      </c>
       <c r="J234" t="inlineStr">
         <is>
-          <t>Parque Faber Castell I</t>
+          <t>Vila Nova Conceição</t>
         </is>
       </c>
       <c r="K234" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 13561-385 </t>
+          <t xml:space="preserve"> 04543-000 </t>
         </is>
       </c>
       <c r="L234" t="inlineStr">
         <is>
-          <t>Gabriel Pinheiro Marto Rodrigues</t>
+          <t>Gabriel Rodrigues</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>POTENZA AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
-        </is>
-      </c>
-      <c r="B235" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 29.936.830/0001-07 </t>
-        </is>
-      </c>
-      <c r="C235" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> contato@potenzacapital.com.br </t>
-        </is>
-      </c>
+          <t>Prosperidade Investimentos Agente Autônomo de investimentos Ltda</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr"/>
+      <c r="C235" t="inlineStr"/>
       <c r="D235" t="inlineStr">
         <is>
-          <t>Avenida Presidente Juscelino Kubitschek, nº 360, conjunto 191</t>
-        </is>
-      </c>
-      <c r="E235" t="inlineStr">
-        <is>
-          <t>(11) 3846-7916</t>
-        </is>
-      </c>
+          <t>Av. Historiador Rubens de Mendonça, 1756 - sala 906</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr"/>
       <c r="F235" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SP </t>
+          <t xml:space="preserve"> MT </t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://www.potenzacapital.com.br/contato </t>
+          <t xml:space="preserve"> - </t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>São Paulo</t>
-        </is>
-      </c>
-      <c r="I235" t="inlineStr">
-        <is>
-          <t>23/07/2020</t>
-        </is>
-      </c>
+          <t>Cuiabá</t>
+        </is>
+      </c>
+      <c r="I235" t="inlineStr"/>
       <c r="J235" t="inlineStr">
         <is>
-          <t>Vila Nova Conceição</t>
+          <t>Alvorada</t>
         </is>
       </c>
       <c r="K235" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 04543-000 </t>
+          <t xml:space="preserve"> 78048-340 </t>
         </is>
       </c>
       <c r="L235" t="inlineStr">
         <is>
-          <t>Gabriel Rodrigues</t>
+          <t>Douglas Sakamiti</t>
         </is>
       </c>
     </row>
@@ -13469,10 +13453,14 @@
       <c r="C236" t="inlineStr"/>
       <c r="D236" t="inlineStr">
         <is>
-          <t>Av. Historiador Rubens de Mendonça, 1756 - sala 906</t>
-        </is>
-      </c>
-      <c r="E236" t="inlineStr"/>
+          <t>Av. Historiador Rubens de Mendonça, 1756, sala 906, Alvorada</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>(11) 3090-6986</t>
+        </is>
+      </c>
       <c r="F236" t="inlineStr">
         <is>
           <t xml:space="preserve"> MT </t>
@@ -13491,7 +13479,7 @@
       <c r="I236" t="inlineStr"/>
       <c r="J236" t="inlineStr">
         <is>
-          <t>Alvorada</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K236" t="inlineStr">
@@ -13515,7 +13503,7 @@
       <c r="C237" t="inlineStr"/>
       <c r="D237" t="inlineStr">
         <is>
-          <t>Av. Historiador Rubens de Mendonça, 1756, sala 906, Alvorada</t>
+          <t>Av. Jornalista Umberto Calderaro Filho, 455, sala 906/907, Edifício Crystal Tower, Adrianópolis</t>
         </is>
       </c>
       <c r="E237" t="inlineStr">
@@ -13525,7 +13513,7 @@
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t xml:space="preserve"> MT </t>
+          <t xml:space="preserve"> AM </t>
         </is>
       </c>
       <c r="G237" t="inlineStr">
@@ -13535,7 +13523,7 @@
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>Cuiabá</t>
+          <t>Manaus</t>
         </is>
       </c>
       <c r="I237" t="inlineStr"/>
@@ -13546,7 +13534,7 @@
       </c>
       <c r="K237" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 78048-340 </t>
+          <t xml:space="preserve"> 69057-015 </t>
         </is>
       </c>
       <c r="L237" t="inlineStr">
@@ -13565,7 +13553,7 @@
       <c r="C238" t="inlineStr"/>
       <c r="D238" t="inlineStr">
         <is>
-          <t>Av. Jornalista Umberto Calderaro Filho, 455, sala 906/907, Edifício Crystal Tower, Adrianópolis</t>
+          <t>Rua Catequese, 725, Sala 11/12/ Vila Guiomar</t>
         </is>
       </c>
       <c r="E238" t="inlineStr">
@@ -13575,7 +13563,7 @@
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AM </t>
+          <t xml:space="preserve"> SP </t>
         </is>
       </c>
       <c r="G238" t="inlineStr">
@@ -13585,7 +13573,7 @@
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Santo André</t>
         </is>
       </c>
       <c r="I238" t="inlineStr"/>
@@ -13596,7 +13584,7 @@
       </c>
       <c r="K238" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 69057-015 </t>
+          <t xml:space="preserve"> 90904-010 </t>
         </is>
       </c>
       <c r="L238" t="inlineStr">
@@ -13615,7 +13603,7 @@
       <c r="C239" t="inlineStr"/>
       <c r="D239" t="inlineStr">
         <is>
-          <t>Rua Catequese, 725, Sala 11/12/ Vila Guiomar</t>
+          <t>Avenida Portugal, 1148, sala B3101/B3103, Setor Marista</t>
         </is>
       </c>
       <c r="E239" t="inlineStr">
@@ -13625,7 +13613,7 @@
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SP </t>
+          <t xml:space="preserve"> GO </t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
@@ -13635,7 +13623,7 @@
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>Santo André</t>
+          <t>Goiânia</t>
         </is>
       </c>
       <c r="I239" t="inlineStr"/>
@@ -13646,7 +13634,7 @@
       </c>
       <c r="K239" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 90904-010 </t>
+          <t xml:space="preserve"> 74150-030 </t>
         </is>
       </c>
       <c r="L239" t="inlineStr">
@@ -13665,14 +13653,10 @@
       <c r="C240" t="inlineStr"/>
       <c r="D240" t="inlineStr">
         <is>
-          <t>Avenida Portugal, 1148, sala B3101/B3103, Setor Marista</t>
-        </is>
-      </c>
-      <c r="E240" t="inlineStr">
-        <is>
-          <t>(11) 3090-6986</t>
-        </is>
-      </c>
+          <t>Avenida Portugal, 1148 - sala B3101/B3103</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr"/>
       <c r="F240" t="inlineStr">
         <is>
           <t xml:space="preserve"> GO </t>
@@ -13691,7 +13675,7 @@
       <c r="I240" t="inlineStr"/>
       <c r="J240" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Set. Marista</t>
         </is>
       </c>
       <c r="K240" t="inlineStr">
@@ -13715,13 +13699,17 @@
       <c r="C241" t="inlineStr"/>
       <c r="D241" t="inlineStr">
         <is>
-          <t>Avenida Portugal, 1148 - sala B3101/B3103</t>
-        </is>
-      </c>
-      <c r="E241" t="inlineStr"/>
+          <t>Avenida Ana Costa, 433/84, Bloco B, Conjunto B, Gonzaga</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>(11) 3090-6986</t>
+        </is>
+      </c>
       <c r="F241" t="inlineStr">
         <is>
-          <t xml:space="preserve"> GO </t>
+          <t xml:space="preserve"> SP </t>
         </is>
       </c>
       <c r="G241" t="inlineStr">
@@ -13731,18 +13719,18 @@
       </c>
       <c r="H241" t="inlineStr">
         <is>
-          <t>Goiânia</t>
+          <t>Santos</t>
         </is>
       </c>
       <c r="I241" t="inlineStr"/>
       <c r="J241" t="inlineStr">
         <is>
-          <t>Set. Marista</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K241" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 74150-030 </t>
+          <t xml:space="preserve"> 11060-003 </t>
         </is>
       </c>
       <c r="L241" t="inlineStr">
@@ -13757,18 +13745,22 @@
           <t>Prosperidade Investimentos Agente Autônomo de investimentos Ltda</t>
         </is>
       </c>
-      <c r="B242" t="inlineStr"/>
-      <c r="C242" t="inlineStr"/>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28.075.248/0001-30 </t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> contato@prosperidadeinvest.com.br </t>
+        </is>
+      </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>Avenida Ana Costa, 433/84, Bloco B, Conjunto B, Gonzaga</t>
-        </is>
-      </c>
-      <c r="E242" t="inlineStr">
-        <is>
-          <t>(11) 3090-6986</t>
-        </is>
-      </c>
+          <t>Av. Domingos de Morais, nº 2187 - sala 613/614 - Torre Paris</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr"/>
       <c r="F242" t="inlineStr">
         <is>
           <t xml:space="preserve"> SP </t>
@@ -13781,18 +13773,22 @@
       </c>
       <c r="H242" t="inlineStr">
         <is>
-          <t>Santos</t>
-        </is>
-      </c>
-      <c r="I242" t="inlineStr"/>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>15/07/2020</t>
+        </is>
+      </c>
       <c r="J242" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Vila Mariana</t>
         </is>
       </c>
       <c r="K242" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 11060-003 </t>
+          <t xml:space="preserve"> 04035-000 </t>
         </is>
       </c>
       <c r="L242" t="inlineStr">
@@ -13807,25 +13803,21 @@
           <t>Prosperidade Investimentos Agente Autônomo de investimentos Ltda</t>
         </is>
       </c>
-      <c r="B243" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 28.075.248/0001-30 </t>
-        </is>
-      </c>
-      <c r="C243" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> contato@prosperidadeinvest.com.br </t>
-        </is>
-      </c>
+      <c r="B243" t="inlineStr"/>
+      <c r="C243" t="inlineStr"/>
       <c r="D243" t="inlineStr">
         <is>
-          <t>Av. Domingos de Morais, nº 2187 - sala 613/614 - Torre Paris</t>
-        </is>
-      </c>
-      <c r="E243" t="inlineStr"/>
+          <t>Av. Ville Roy, 4390, Nossa Senhora Aparecida</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>(11) 3090-6986</t>
+        </is>
+      </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SP </t>
+          <t xml:space="preserve"> RR </t>
         </is>
       </c>
       <c r="G243" t="inlineStr">
@@ -13835,22 +13827,18 @@
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>São Paulo</t>
-        </is>
-      </c>
-      <c r="I243" t="inlineStr">
-        <is>
-          <t>15/07/2020</t>
-        </is>
-      </c>
+          <t>Boa Vista</t>
+        </is>
+      </c>
+      <c r="I243" t="inlineStr"/>
       <c r="J243" t="inlineStr">
         <is>
-          <t>Vila Mariana</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K243" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 04035-000 </t>
+          <t xml:space="preserve"> 69306-405 </t>
         </is>
       </c>
       <c r="L243" t="inlineStr">
@@ -13869,17 +13857,13 @@
       <c r="C244" t="inlineStr"/>
       <c r="D244" t="inlineStr">
         <is>
-          <t>Av. Ville Roy, 4390, Nossa Senhora Aparecida</t>
-        </is>
-      </c>
-      <c r="E244" t="inlineStr">
-        <is>
-          <t>(11) 3090-6986</t>
-        </is>
-      </c>
+          <t>Av. Jornalista Umberto Calderaro Filho, 455 - sala 906/907 - Ed Crystal Tower</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr"/>
       <c r="F244" t="inlineStr">
         <is>
-          <t xml:space="preserve"> RR </t>
+          <t xml:space="preserve"> AM </t>
         </is>
       </c>
       <c r="G244" t="inlineStr">
@@ -13889,18 +13873,18 @@
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>Boa Vista</t>
+          <t>Manaus</t>
         </is>
       </c>
       <c r="I244" t="inlineStr"/>
       <c r="J244" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Adrianópolis</t>
         </is>
       </c>
       <c r="K244" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 69306-405 </t>
+          <t xml:space="preserve"> 69057-015 </t>
         </is>
       </c>
       <c r="L244" t="inlineStr">
@@ -13919,13 +13903,13 @@
       <c r="C245" t="inlineStr"/>
       <c r="D245" t="inlineStr">
         <is>
-          <t>Av. Jornalista Umberto Calderaro Filho, 455 - sala 906/907 - Ed Crystal Tower</t>
+          <t>Av. Republica do Líbano, 251 - sala 1303 - torre B</t>
         </is>
       </c>
       <c r="E245" t="inlineStr"/>
       <c r="F245" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AM </t>
+          <t xml:space="preserve"> PE </t>
         </is>
       </c>
       <c r="G245" t="inlineStr">
@@ -13935,18 +13919,18 @@
       </c>
       <c r="H245" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Recife</t>
         </is>
       </c>
       <c r="I245" t="inlineStr"/>
       <c r="J245" t="inlineStr">
         <is>
-          <t>Adrianópolis</t>
+          <t>Pina</t>
         </is>
       </c>
       <c r="K245" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 69057-015 </t>
+          <t xml:space="preserve"> 51110-160 </t>
         </is>
       </c>
       <c r="L245" t="inlineStr">
@@ -13965,13 +13949,13 @@
       <c r="C246" t="inlineStr"/>
       <c r="D246" t="inlineStr">
         <is>
-          <t>Av. Republica do Líbano, 251 - sala 1303 - torre B</t>
+          <t>Av. Ville Roy, 4390</t>
         </is>
       </c>
       <c r="E246" t="inlineStr"/>
       <c r="F246" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PE </t>
+          <t xml:space="preserve"> RR </t>
         </is>
       </c>
       <c r="G246" t="inlineStr">
@@ -13981,18 +13965,18 @@
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Boa Vista</t>
         </is>
       </c>
       <c r="I246" t="inlineStr"/>
       <c r="J246" t="inlineStr">
         <is>
-          <t>Pina</t>
+          <t>Nossa Senhora Aparecida</t>
         </is>
       </c>
       <c r="K246" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 51110-160 </t>
+          <t xml:space="preserve"> 69306-405 </t>
         </is>
       </c>
       <c r="L246" t="inlineStr">
@@ -14011,13 +13995,13 @@
       <c r="C247" t="inlineStr"/>
       <c r="D247" t="inlineStr">
         <is>
-          <t>Av. Ville Roy, 4390</t>
+          <t>SHS Quadra 6, conjunto A, bloco A, S/N, Ed. Brasil 21 - sala 806</t>
         </is>
       </c>
       <c r="E247" t="inlineStr"/>
       <c r="F247" t="inlineStr">
         <is>
-          <t xml:space="preserve"> RR </t>
+          <t xml:space="preserve"> DF </t>
         </is>
       </c>
       <c r="G247" t="inlineStr">
@@ -14027,18 +14011,18 @@
       </c>
       <c r="H247" t="inlineStr">
         <is>
-          <t>Boa Vista</t>
+          <t>Brasília</t>
         </is>
       </c>
       <c r="I247" t="inlineStr"/>
       <c r="J247" t="inlineStr">
         <is>
-          <t>Nossa Senhora Aparecida</t>
+          <t>Asa Sul</t>
         </is>
       </c>
       <c r="K247" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 69306-405 </t>
+          <t xml:space="preserve"> 70316-102 </t>
         </is>
       </c>
       <c r="L247" t="inlineStr">
@@ -14057,13 +14041,17 @@
       <c r="C248" t="inlineStr"/>
       <c r="D248" t="inlineStr">
         <is>
-          <t>SHS Quadra 6, conjunto A, bloco A, S/N, Ed. Brasil 21 - sala 806</t>
-        </is>
-      </c>
-      <c r="E248" t="inlineStr"/>
+          <t>Avenida Afonso Pena, 4875, sala 2102, Santa Fé</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>(11) 3090-6986</t>
+        </is>
+      </c>
       <c r="F248" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DF </t>
+          <t xml:space="preserve"> MS </t>
         </is>
       </c>
       <c r="G248" t="inlineStr">
@@ -14073,18 +14061,18 @@
       </c>
       <c r="H248" t="inlineStr">
         <is>
-          <t>Brasília</t>
+          <t>Campo Grande</t>
         </is>
       </c>
       <c r="I248" t="inlineStr"/>
       <c r="J248" t="inlineStr">
         <is>
-          <t>Asa Sul</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K248" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 70316-102 </t>
+          <t xml:space="preserve"> 79031-010 </t>
         </is>
       </c>
       <c r="L248" t="inlineStr">
@@ -14103,7 +14091,7 @@
       <c r="C249" t="inlineStr"/>
       <c r="D249" t="inlineStr">
         <is>
-          <t>Avenida Afonso Pena, 4875, sala 2102, Santa Fé</t>
+          <t>SHS Quadra 6, conjunto A, bloco A, S/N, Edifício Brasil 21, sala 806, Asa Sul</t>
         </is>
       </c>
       <c r="E249" t="inlineStr">
@@ -14113,7 +14101,7 @@
       </c>
       <c r="F249" t="inlineStr">
         <is>
-          <t xml:space="preserve"> MS </t>
+          <t xml:space="preserve"> DF </t>
         </is>
       </c>
       <c r="G249" t="inlineStr">
@@ -14123,7 +14111,7 @@
       </c>
       <c r="H249" t="inlineStr">
         <is>
-          <t>Campo Grande</t>
+          <t>Brasília</t>
         </is>
       </c>
       <c r="I249" t="inlineStr"/>
@@ -14134,7 +14122,7 @@
       </c>
       <c r="K249" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 79031-010 </t>
+          <t xml:space="preserve"> 70316-102 </t>
         </is>
       </c>
       <c r="L249" t="inlineStr">
@@ -14153,7 +14141,7 @@
       <c r="C250" t="inlineStr"/>
       <c r="D250" t="inlineStr">
         <is>
-          <t>SHS Quadra 6, conjunto A, bloco A, S/N, Edifício Brasil 21, sala 806, Asa Sul</t>
+          <t>Av. Republica do Líbano, 251, sala 1303, Torre B, Bairro Pina</t>
         </is>
       </c>
       <c r="E250" t="inlineStr">
@@ -14163,7 +14151,7 @@
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DF </t>
+          <t xml:space="preserve"> PE </t>
         </is>
       </c>
       <c r="G250" t="inlineStr">
@@ -14173,7 +14161,7 @@
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>Brasília</t>
+          <t>Recife</t>
         </is>
       </c>
       <c r="I250" t="inlineStr"/>
@@ -14184,7 +14172,7 @@
       </c>
       <c r="K250" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 70316-102 </t>
+          <t xml:space="preserve"> 51110-160 </t>
         </is>
       </c>
       <c r="L250" t="inlineStr">
@@ -14196,24 +14184,32 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Prosperidade Investimentos Agente Autônomo de investimentos Ltda</t>
-        </is>
-      </c>
-      <c r="B251" t="inlineStr"/>
-      <c r="C251" t="inlineStr"/>
+          <t>RAUL CARVALHO IV - AGENTE AUTONOMO DE INVESTIMENTO S/S</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 40.202.799/0001-13 </t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> investimentos@raulcarvalhoiv.com.br </t>
+        </is>
+      </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>Av. Republica do Líbano, 251, sala 1303, Torre B, Bairro Pina</t>
+          <t>Rua Pamplona, nº 1551 - Apt 1609,</t>
         </is>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>(11) 3090-6986</t>
+          <t>(11) 3185-6959</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PE </t>
+          <t xml:space="preserve"> SP </t>
         </is>
       </c>
       <c r="G251" t="inlineStr">
@@ -14223,55 +14219,59 @@
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>Recife</t>
-        </is>
-      </c>
-      <c r="I251" t="inlineStr"/>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>22/02/2021</t>
+        </is>
+      </c>
       <c r="J251" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Jardim Paulista</t>
         </is>
       </c>
       <c r="K251" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 51110-160 </t>
+          <t xml:space="preserve"> 14050-020 </t>
         </is>
       </c>
       <c r="L251" t="inlineStr">
         <is>
-          <t>Douglas Sakamiti</t>
+          <t>Raul Carvalho IV</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>RAUL CARVALHO IV - AGENTE AUTONOMO DE INVESTIMENTO S/S</t>
+          <t>REGATA AGENTE AUTONOMO DE INVESTIMENTOS FINANCEIROS S/S LTDA</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 40.202.799/0001-13 </t>
+          <t xml:space="preserve"> 15.828.426/0001-05 </t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t xml:space="preserve"> investimentos@raulcarvalhoiv.com.br </t>
+          <t xml:space="preserve"> nathaniel@regatainvestimentos.com </t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>Rua Pamplona, nº 1551 - Apt 1609,</t>
+          <t>SCN Quadra 2 Bloco A, 190 - sala 503 - Ed. Corporate Financial Center Parte Z</t>
         </is>
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>(11) 3185-6959</t>
+          <t>(61) 3521-5345</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SP </t>
+          <t xml:space="preserve"> DF </t>
         </is>
       </c>
       <c r="G252" t="inlineStr">
@@ -14281,54 +14281,46 @@
       </c>
       <c r="H252" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Brasilia</t>
         </is>
       </c>
       <c r="I252" t="inlineStr">
         <is>
-          <t>22/02/2021</t>
+          <t>22/10/2020</t>
         </is>
       </c>
       <c r="J252" t="inlineStr">
         <is>
-          <t>Jardim Paulista</t>
+          <t>Asa Norte</t>
         </is>
       </c>
       <c r="K252" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 14050-020 </t>
+          <t xml:space="preserve"> 70712-900 </t>
         </is>
       </c>
       <c r="L252" t="inlineStr">
         <is>
-          <t>Raul Carvalho IV</t>
+          <t>NATHANIEL SENOS BLOOMFIELD</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>REGATA AGENTE AUTONOMO DE INVESTIMENTOS FINANCEIROS S/S LTDA</t>
-        </is>
-      </c>
-      <c r="B253" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 15.828.426/0001-05 </t>
-        </is>
-      </c>
-      <c r="C253" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> nathaniel@regatainvestimentos.com </t>
-        </is>
-      </c>
+          <t>RENOVA INVEST AGENTES AUTONOMOS DE INVESTIMENTOS LTDA</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr"/>
+      <c r="C253" t="inlineStr"/>
       <c r="D253" t="inlineStr">
         <is>
-          <t>SCN Quadra 2 Bloco A, 190 - sala 503 - Ed. Corporate Financial Center Parte Z</t>
+          <t>Quadra SHS Quadra 6, conjunto A, bloco C, salas 1111, 1112 e 1113</t>
         </is>
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>(61) 3521-5345</t>
+          <t>(61) 3963-0005</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -14338,32 +14330,28 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t xml:space="preserve"> https://renovainvest.com.br/ </t>
         </is>
       </c>
       <c r="H253" t="inlineStr">
         <is>
-          <t>Brasilia</t>
-        </is>
-      </c>
-      <c r="I253" t="inlineStr">
-        <is>
-          <t>22/10/2020</t>
-        </is>
-      </c>
+          <t>Brasília</t>
+        </is>
+      </c>
+      <c r="I253" t="inlineStr"/>
       <c r="J253" t="inlineStr">
         <is>
-          <t>Asa Norte</t>
+          <t>Asa Sul</t>
         </is>
       </c>
       <c r="K253" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 70712-900 </t>
+          <t xml:space="preserve"> 70316-000 </t>
         </is>
       </c>
       <c r="L253" t="inlineStr">
         <is>
-          <t>NATHANIEL SENOS BLOOMFIELD</t>
+          <t>Bruno Ismar</t>
         </is>
       </c>
     </row>
@@ -14373,47 +14361,59 @@
           <t>RENOVA INVEST AGENTES AUTONOMOS DE INVESTIMENTOS LTDA</t>
         </is>
       </c>
-      <c r="B254" t="inlineStr"/>
-      <c r="C254" t="inlineStr"/>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 19.419.958/0001-40 </t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> bruno.ismar@renovainvest.com.br </t>
+        </is>
+      </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>Quadra SHS Quadra 6, conjunto A, bloco C, salas 1111, 1112 e 1113</t>
+          <t>Rua Fradique Coutinho, 50, Conjuntos 53 e 54</t>
         </is>
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>(61) 3963-0005</t>
+          <t>(11) 3192-3882</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DF </t>
+          <t xml:space="preserve"> SP </t>
         </is>
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://renovainvest.com.br/ </t>
+          <t xml:space="preserve"> https://www.renovainvest.com.br/ </t>
         </is>
       </c>
       <c r="H254" t="inlineStr">
         <is>
-          <t>Brasília</t>
-        </is>
-      </c>
-      <c r="I254" t="inlineStr"/>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="I254" t="inlineStr">
+        <is>
+          <t>21/12/2018</t>
+        </is>
+      </c>
       <c r="J254" t="inlineStr">
         <is>
-          <t>Asa Sul</t>
+          <t>Pinheiros</t>
         </is>
       </c>
       <c r="K254" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 70316-000 </t>
+          <t xml:space="preserve"> 05416-000 </t>
         </is>
       </c>
       <c r="L254" t="inlineStr">
         <is>
-          <t>Bruno Ismar</t>
+          <t>Bruno Ismar da Silva</t>
         </is>
       </c>
     </row>
@@ -14423,26 +14423,14 @@
           <t>RENOVA INVEST AGENTES AUTONOMOS DE INVESTIMENTOS LTDA</t>
         </is>
       </c>
-      <c r="B255" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 19.419.958/0001-40 </t>
-        </is>
-      </c>
-      <c r="C255" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> bruno.ismar@renovainvest.com.br </t>
-        </is>
-      </c>
+      <c r="B255" t="inlineStr"/>
+      <c r="C255" t="inlineStr"/>
       <c r="D255" t="inlineStr">
         <is>
-          <t>Rua Fradique Coutinho, 50, Conjuntos 53 e 54</t>
-        </is>
-      </c>
-      <c r="E255" t="inlineStr">
-        <is>
-          <t>(11) 3192-3882</t>
-        </is>
-      </c>
+          <t>Rua Cantagalo, nº 74, conjuntos 1806 a 1810</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr"/>
       <c r="F255" t="inlineStr">
         <is>
           <t xml:space="preserve"> SP </t>
@@ -14450,7 +14438,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://www.renovainvest.com.br/ </t>
+          <t xml:space="preserve"> https://renovainvest.com.br/ </t>
         </is>
       </c>
       <c r="H255" t="inlineStr">
@@ -14458,19 +14446,15 @@
           <t>São Paulo</t>
         </is>
       </c>
-      <c r="I255" t="inlineStr">
-        <is>
-          <t>21/12/2018</t>
-        </is>
-      </c>
+      <c r="I255" t="inlineStr"/>
       <c r="J255" t="inlineStr">
         <is>
-          <t>Pinheiros</t>
+          <t>Vila Gomes Cardim</t>
         </is>
       </c>
       <c r="K255" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 05416-000 </t>
+          <t xml:space="preserve"> 03319-900 </t>
         </is>
       </c>
       <c r="L255" t="inlineStr">
@@ -14489,13 +14473,13 @@
       <c r="C256" t="inlineStr"/>
       <c r="D256" t="inlineStr">
         <is>
-          <t>Rua Cantagalo, nº 74, conjuntos 1806 a 1810</t>
+          <t>Rua Padre Anchieta, nº 2050, 24º andar, salas 2405, 2406 e 2407</t>
         </is>
       </c>
       <c r="E256" t="inlineStr"/>
       <c r="F256" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SP </t>
+          <t xml:space="preserve"> PR </t>
         </is>
       </c>
       <c r="G256" t="inlineStr">
@@ -14505,18 +14489,18 @@
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Curitiba</t>
         </is>
       </c>
       <c r="I256" t="inlineStr"/>
       <c r="J256" t="inlineStr">
         <is>
-          <t>Vila Gomes Cardim</t>
+          <t>Bigorrilho</t>
         </is>
       </c>
       <c r="K256" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 03319-900 </t>
+          <t xml:space="preserve"> 80730-001 </t>
         </is>
       </c>
       <c r="L256" t="inlineStr">
@@ -14535,13 +14519,13 @@
       <c r="C257" t="inlineStr"/>
       <c r="D257" t="inlineStr">
         <is>
-          <t>Rua Padre Anchieta, nº 2050, 24º andar, salas 2405, 2406 e 2407</t>
+          <t>Rua Sete de Setembro, nº 777, sala 509</t>
         </is>
       </c>
       <c r="E257" t="inlineStr"/>
       <c r="F257" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PR </t>
+          <t xml:space="preserve"> SC </t>
         </is>
       </c>
       <c r="G257" t="inlineStr">
@@ -14551,18 +14535,18 @@
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>Blumenau</t>
         </is>
       </c>
       <c r="I257" t="inlineStr"/>
       <c r="J257" t="inlineStr">
         <is>
-          <t>Bigorrilho</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="K257" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 80730-001 </t>
+          <t xml:space="preserve"> 89010-203 </t>
         </is>
       </c>
       <c r="L257" t="inlineStr">
@@ -14581,13 +14565,13 @@
       <c r="C258" t="inlineStr"/>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Rua Sete de Setembro, nº 777, sala 509</t>
+          <t>Avenida Nossa Senhora de Fátima, nº 3-97, Lote 15, Quadra 11</t>
         </is>
       </c>
       <c r="E258" t="inlineStr"/>
       <c r="F258" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SC </t>
+          <t xml:space="preserve"> SP </t>
         </is>
       </c>
       <c r="G258" t="inlineStr">
@@ -14597,18 +14581,18 @@
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>Blumenau</t>
+          <t>Bauru</t>
         </is>
       </c>
       <c r="I258" t="inlineStr"/>
       <c r="J258" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Jardim América</t>
         </is>
       </c>
       <c r="K258" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 89010-203 </t>
+          <t xml:space="preserve"> 17017-337 </t>
         </is>
       </c>
       <c r="L258" t="inlineStr">
@@ -14620,17 +14604,29 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>RENOVA INVEST AGENTES AUTONOMOS DE INVESTIMENTOS LTDA</t>
-        </is>
-      </c>
-      <c r="B259" t="inlineStr"/>
-      <c r="C259" t="inlineStr"/>
+          <t>RUBI AGENTE AUTONOMO DE INVESTIMENTOS S/S LTDA</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 46.002.875/0001-23 </t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> atendimento@rubiinvestimentos.com.br </t>
+        </is>
+      </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>Avenida Nossa Senhora de Fátima, nº 3-97, Lote 15, Quadra 11</t>
-        </is>
-      </c>
-      <c r="E259" t="inlineStr"/>
+          <t>Alameda Rio Negro, 1084 sala A 31</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>(11) 3181-8780</t>
+        </is>
+      </c>
       <c r="F259" t="inlineStr">
         <is>
           <t xml:space="preserve"> SP </t>
@@ -14638,90 +14634,78 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://renovainvest.com.br/ </t>
+          <t xml:space="preserve"> www.rubiinvestimentos.com.br </t>
         </is>
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>Bauru</t>
-        </is>
-      </c>
-      <c r="I259" t="inlineStr"/>
+          <t>Barueri</t>
+        </is>
+      </c>
+      <c r="I259" t="inlineStr">
+        <is>
+          <t>10/05/2022</t>
+        </is>
+      </c>
       <c r="J259" t="inlineStr">
         <is>
-          <t>Jardim América</t>
+          <t>Alphaville</t>
         </is>
       </c>
       <c r="K259" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 17017-337 </t>
+          <t xml:space="preserve"> 06472-001 </t>
         </is>
       </c>
       <c r="L259" t="inlineStr">
         <is>
-          <t>Bruno Ismar da Silva</t>
+          <t>Anna Luiza Turqueti Vieira</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>RUBI AGENTE AUTONOMO DE INVESTIMENTOS S/S LTDA</t>
-        </is>
-      </c>
-      <c r="B260" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 46.002.875/0001-23 </t>
-        </is>
-      </c>
-      <c r="C260" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> atendimento@rubiinvestimentos.com.br </t>
-        </is>
-      </c>
+          <t>SACRE - AGENTE AUTONOMO DE INVESTIMENTO S/S LTDA</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr"/>
+      <c r="C260" t="inlineStr"/>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Alameda Rio Negro, 1084 sala A 31</t>
-        </is>
-      </c>
-      <c r="E260" t="inlineStr">
-        <is>
-          <t>(11) 3181-8780</t>
-        </is>
-      </c>
+          <t>Avenida Carneiro Leão, Nº 563, 11º andar</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr"/>
       <c r="F260" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SP </t>
+          <t xml:space="preserve"> PR </t>
         </is>
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t xml:space="preserve"> www.rubiinvestimentos.com.br </t>
+          <t xml:space="preserve"> - </t>
         </is>
       </c>
       <c r="H260" t="inlineStr">
         <is>
-          <t>Barueri</t>
-        </is>
-      </c>
-      <c r="I260" t="inlineStr">
-        <is>
-          <t>10/05/2022</t>
-        </is>
-      </c>
+          <t>Maringá</t>
+        </is>
+      </c>
+      <c r="I260" t="inlineStr"/>
       <c r="J260" t="inlineStr">
         <is>
-          <t>Alphaville</t>
+          <t>Zona Armazém</t>
         </is>
       </c>
       <c r="K260" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 06472-001 </t>
+          <t xml:space="preserve"> 87014-010 </t>
         </is>
       </c>
       <c r="L260" t="inlineStr">
         <is>
-          <t>Anna Luiza Turqueti Vieira</t>
+          <t>HELIO AUGUSTO RANIERI</t>
         </is>
       </c>
     </row>
@@ -14731,11 +14715,19 @@
           <t>SACRE - AGENTE AUTONOMO DE INVESTIMENTO S/S LTDA</t>
         </is>
       </c>
-      <c r="B261" t="inlineStr"/>
-      <c r="C261" t="inlineStr"/>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28.811.973/0001-20 </t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>Avenida Carneiro Leão, Nº 563, 11º andar</t>
+          <t>AV XV DE NOVEMBRO 171, SALA 01</t>
         </is>
       </c>
       <c r="E261" t="inlineStr"/>
@@ -14746,23 +14738,27 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t xml:space="preserve"> https://sacreinvestimentos.com.br/ </t>
         </is>
       </c>
       <c r="H261" t="inlineStr">
         <is>
-          <t>Maringá</t>
-        </is>
-      </c>
-      <c r="I261" t="inlineStr"/>
+          <t>MARINGA</t>
+        </is>
+      </c>
+      <c r="I261" t="inlineStr">
+        <is>
+          <t>29/09/2021</t>
+        </is>
+      </c>
       <c r="J261" t="inlineStr">
         <is>
-          <t>Zona Armazém</t>
+          <t>ZONA 01</t>
         </is>
       </c>
       <c r="K261" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 87014-010 </t>
+          <t xml:space="preserve"> 87013-904 </t>
         </is>
       </c>
       <c r="L261" t="inlineStr">
@@ -14774,430 +14770,434 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>SACRE - AGENTE AUTONOMO DE INVESTIMENTO S/S LTDA</t>
+          <t>SAFIRA INVESTIMENTOS AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 28.811.973/0001-20 </t>
+          <t xml:space="preserve"> 42.599.433/0001-55 </t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t xml:space="preserve"> caioesteves@safirainvestimentos.com </t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>AV XV DE NOVEMBRO 171, SALA 01</t>
-        </is>
-      </c>
-      <c r="E262" t="inlineStr"/>
+          <t>Rua Paraíba, 550 - 9° andar</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>(31) 3268-9215</t>
+        </is>
+      </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PR </t>
+          <t xml:space="preserve"> MG </t>
         </is>
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://sacreinvestimentos.com.br/ </t>
+          <t xml:space="preserve"> www.safirainvestimentos.com </t>
         </is>
       </c>
       <c r="H262" t="inlineStr">
         <is>
-          <t>MARINGA</t>
+          <t>Belo Horizonte</t>
         </is>
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>29/09/2021</t>
+          <t>15/07/2021</t>
         </is>
       </c>
       <c r="J262" t="inlineStr">
         <is>
-          <t>ZONA 01</t>
+          <t>Savassi</t>
         </is>
       </c>
       <c r="K262" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 87013-904 </t>
+          <t xml:space="preserve"> 30130-140 </t>
         </is>
       </c>
       <c r="L262" t="inlineStr">
         <is>
-          <t>HELIO AUGUSTO RANIERI</t>
+          <t>Caio Esteves</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>SAFIRA INVESTIMENTOS AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
+          <t>SEED CAPITAL PARTNERS AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 42.599.433/0001-55 </t>
+          <t xml:space="preserve"> 42.175.759/0001-55 </t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t xml:space="preserve"> caioesteves@safirainvestimentos.com </t>
+          <t xml:space="preserve"> contato@seedpar.com.br </t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Rua Paraíba, 550 - 9° andar</t>
+          <t>R DO ROCIO, 350, CONJ 11</t>
         </is>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>(31) 3268-9215</t>
+          <t>(11) 2147-0450</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t xml:space="preserve"> MG </t>
+          <t xml:space="preserve"> SP </t>
         </is>
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t xml:space="preserve"> www.safirainvestimentos.com </t>
+          <t xml:space="preserve"> www.obbcapital.com.br </t>
         </is>
       </c>
       <c r="H263" t="inlineStr">
         <is>
-          <t>Belo Horizonte</t>
+          <t>São Paulo</t>
         </is>
       </c>
       <c r="I263" t="inlineStr">
         <is>
-          <t>15/07/2021</t>
+          <t>23/06/2021</t>
         </is>
       </c>
       <c r="J263" t="inlineStr">
         <is>
-          <t>Savassi</t>
+          <t>VILA OLIMPIA</t>
         </is>
       </c>
       <c r="K263" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 30130-140 </t>
+          <t xml:space="preserve"> 04552-000 </t>
         </is>
       </c>
       <c r="L263" t="inlineStr">
         <is>
-          <t>Caio Esteves</t>
+          <t>GUILHERME REBOUCAS DE OLIVEIRA</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>SEED CAPITAL PARTNERS AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
+          <t>SEGMENTO INTERMEDIADORA DE AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 42.175.759/0001-55 </t>
+          <t xml:space="preserve"> 02.499.240/0001-08 </t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@seedpar.com.br </t>
+          <t xml:space="preserve"> institucional@segmentobsb.com.br </t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>R DO ROCIO, 350, CONJ 11</t>
+          <t>SMPW Quadra 15 Conjunto 1, 4 - sala 1309</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>(11) 2147-0450</t>
+          <t>(61) 3326-3832</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SP </t>
+          <t xml:space="preserve"> DF </t>
         </is>
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t xml:space="preserve"> www.obbcapital.com.br </t>
+          <t xml:space="preserve"> https://www.segmentobsb.com.br </t>
         </is>
       </c>
       <c r="H264" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Brasilia</t>
         </is>
       </c>
       <c r="I264" t="inlineStr">
         <is>
-          <t>23/06/2021</t>
+          <t>24/11/2020</t>
         </is>
       </c>
       <c r="J264" t="inlineStr">
         <is>
-          <t>VILA OLIMPIA</t>
+          <t>Park Way</t>
         </is>
       </c>
       <c r="K264" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 04552-000 </t>
+          <t xml:space="preserve"> 71741-501 </t>
         </is>
       </c>
       <c r="L264" t="inlineStr">
         <is>
-          <t>GUILHERME REBOUCAS DE OLIVEIRA</t>
+          <t>PEDRO FELIPE BORGES</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>SEGMENTO INTERMEDIADORA DE AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
+          <t>SIGMA AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 02.499.240/0001-08 </t>
+          <t xml:space="preserve"> 38.006.299/0001-64 </t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t xml:space="preserve"> institucional@segmentobsb.com.br </t>
+          <t xml:space="preserve"> contato@sigmainvest.com.br </t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>SMPW Quadra 15 Conjunto 1, 4 - sala 1309</t>
+          <t>Rua Sergipe 853 - 4° Andar - Sala 01</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>(61) 3326-3832</t>
+          <t>(31) 3268-9293</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DF </t>
+          <t xml:space="preserve"> MG </t>
         </is>
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://www.segmentobsb.com.br </t>
+          <t xml:space="preserve"> www.sigmainvest.com.br </t>
         </is>
       </c>
       <c r="H265" t="inlineStr">
         <is>
-          <t>Brasilia</t>
+          <t>Belo Horizonte</t>
         </is>
       </c>
       <c r="I265" t="inlineStr">
         <is>
-          <t>24/11/2020</t>
+          <t>05/01/2021</t>
         </is>
       </c>
       <c r="J265" t="inlineStr">
         <is>
-          <t>Park Way</t>
+          <t>Savassi</t>
         </is>
       </c>
       <c r="K265" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 71741-501 </t>
+          <t xml:space="preserve"> 30130-171 </t>
         </is>
       </c>
       <c r="L265" t="inlineStr">
         <is>
-          <t>PEDRO FELIPE BORGES</t>
+          <t>Cristiano de Jesus Souto</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>SIGMA AGENTE AUTONOMO DE INVESTIMENTOS LTDA</t>
+          <t>SKG INVESTIMENTOS AGENTE AUTONOMO DE INVESTIMENTOS</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 38.006.299/0001-64 </t>
+          <t xml:space="preserve"> 34.573.542/0001-75 </t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@sigmainvest.com.br </t>
+          <t xml:space="preserve"> gabriel.paiva@skginvestimentos.com.br </t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Rua Sergipe 853 - 4° Andar - Sala 01</t>
+          <t>Rua Jerônimo da Veiga, 45, 6º andar</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>(31) 3268-9293</t>
+          <t>(11) 3077-0101</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t xml:space="preserve"> MG </t>
+          <t xml:space="preserve"> SP </t>
         </is>
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t xml:space="preserve"> www.sigmainvest.com.br </t>
+          <t xml:space="preserve"> - </t>
         </is>
       </c>
       <c r="H266" t="inlineStr">
         <is>
-          <t>Belo Horizonte</t>
+          <t>São Paulo</t>
         </is>
       </c>
       <c r="I266" t="inlineStr">
         <is>
-          <t>05/01/2021</t>
+          <t>14/11/2019</t>
         </is>
       </c>
       <c r="J266" t="inlineStr">
         <is>
-          <t>Savassi</t>
+          <t>Itaim Bibi</t>
         </is>
       </c>
       <c r="K266" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 30130-171 </t>
+          <t xml:space="preserve"> 04536-000 </t>
         </is>
       </c>
       <c r="L266" t="inlineStr">
         <is>
-          <t>Cristiano de Jesus Souto</t>
+          <t>Gabriel Marques de Paiva</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>SKG INVESTIMENTOS AGENTE AUTONOMO DE INVESTIMENTOS</t>
+          <t>SLR AGENTE AUTONOMO DE INVESTIMENTOS EIRELI</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 34.573.542/0001-75 </t>
+          <t xml:space="preserve"> 13.204.239/0001-25 </t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t xml:space="preserve"> gabriel.paiva@skginvestimentos.com.br </t>
+          <t xml:space="preserve"> jorny@slrinvestimentos.com.br </t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Rua Jerônimo da Veiga, 45, 6º andar</t>
+          <t>Rua Visconde do Rio Branco, 1717 - cj 53</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>(11) 3077-0101</t>
+          <t>(48) 3226-8173</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SP </t>
+          <t xml:space="preserve"> PR </t>
         </is>
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t xml:space="preserve"> www.slrinvestimentos.com.br </t>
         </is>
       </c>
       <c r="H267" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Curitiba</t>
         </is>
       </c>
       <c r="I267" t="inlineStr">
         <is>
-          <t>14/11/2019</t>
+          <t>14/11/2022</t>
         </is>
       </c>
       <c r="J267" t="inlineStr">
         <is>
-          <t>Itaim Bibi</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="K267" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 04536-000 </t>
+          <t xml:space="preserve"> 80420-210 </t>
         </is>
       </c>
       <c r="L267" t="inlineStr">
         <is>
-          <t>Gabriel Marques de Paiva</t>
+          <t>JORNY FABIANO BROTTO</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>SLR AGENTE AUTONOMO DE INVESTIMENTOS EIRELI</t>
+          <t>SOMMA ASSESSORIA DE INVESTIMENTOS S/S LTDA</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 13.204.239/0001-25 </t>
+          <t xml:space="preserve"> 29.724.240/0001-10 </t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t xml:space="preserve"> jorny@slrinvestimentos.com.br </t>
+          <t xml:space="preserve"> investimentos@pluginvestimentos.com.br </t>
         </is>
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Rua Visconde do Rio Branco, 1717 - cj 53</t>
+          <t>Rua Lauro Linhares, 2010, Sala 709 - Bloco A</t>
         </is>
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>(48) 3226-8173</t>
+          <t>(48) 3207-6579</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PR </t>
+          <t xml:space="preserve"> SC </t>
         </is>
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t xml:space="preserve"> www.slrinvestimentos.com.br </t>
+          <t xml:space="preserve"> - </t>
         </is>
       </c>
       <c r="H268" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>Florianópolis</t>
         </is>
       </c>
       <c r="I268" t="inlineStr">
         <is>
-          <t>14/11/2022</t>
+          <t>07/02/2022</t>
         </is>
       </c>
       <c r="J268" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Trindade</t>
         </is>
       </c>
       <c r="K268" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 80420-210 </t>
+          <t xml:space="preserve"> 88036-002 </t>
         </is>
       </c>
       <c r="L268" t="inlineStr">
         <is>
-          <t>JORNY FABIANO BROTTO</t>
+          <t>JOÃO FELIPE DA SILVA FRANDOLOZO</t>
         </is>
       </c>
     </row>

</xml_diff>